<commit_message>
Change to age definition
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Human-being_Defs.xlsx
+++ b/inputs/AddictO_Human-being_Defs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\User3\Work\Github\addiction-ontology\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saeed\Documents\GitHub\addiction-ontology\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="944">
   <si>
     <t>ID</t>
   </si>
@@ -2700,9 +2700,6 @@
     <t>Agent</t>
   </si>
   <si>
-    <t>ICO:0000220</t>
-  </si>
-  <si>
     <t>A material entity  that is either a human being, an aggregate of humans or an organisation and that has the capability of intentionality.</t>
   </si>
   <si>
@@ -2718,9 +2715,6 @@
     <t>A time quality inhering in a bearer by virtue of how much time elapsed between birth and a certain point.</t>
   </si>
   <si>
-    <t>Time [PATO:0000165]</t>
-  </si>
-  <si>
     <t>Data item</t>
   </si>
   <si>
@@ -2863,12 +2857,15 @@
   </si>
   <si>
     <t>Subjective sensation</t>
+  </si>
+  <si>
+    <t>Physical quality; PATO:0001018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3098,7 +3095,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3399,8 +3396,8 @@
   <dimension ref="A1:S679"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46:XFD46"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,7 +3476,7 @@
         <v>148</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3487,7 +3484,7 @@
         <v>153</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>3</v>
@@ -3513,7 +3510,7 @@
         <v>155</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>589</v>
@@ -3525,7 +3522,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>156</v>
@@ -3685,19 +3682,22 @@
         <v>165</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>896</v>
+        <v>943</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G12" s="13" t="s">
+        <v>892</v>
+      </c>
       <c r="H12" s="8" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="J12" s="14"/>
       <c r="N12" s="13">
@@ -3709,9 +3709,7 @@
       <c r="R12" s="14"/>
     </row>
     <row r="13" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>890</v>
-      </c>
+      <c r="A13" s="8"/>
       <c r="B13" s="13" t="s">
         <v>166</v>
       </c>
@@ -4281,7 +4279,7 @@
         <v>203</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D45" s="13" t="s">
         <v>204</v>
@@ -4313,7 +4311,7 @@
         <v>81</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="E46" s="21" t="s">
         <v>58</v>
@@ -4333,7 +4331,7 @@
       </c>
       <c r="O46" s="21"/>
       <c r="P46" s="21" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="Q46" s="20"/>
       <c r="R46" s="20"/>
@@ -5832,7 +5830,7 @@
         <v>295</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D128" s="11" t="s">
         <v>860</v>
@@ -5963,10 +5961,10 @@
         <v>313</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E134" s="20" t="s">
         <v>63</v>
@@ -5984,7 +5982,7 @@
       <c r="N134" s="20"/>
       <c r="O134" s="20"/>
       <c r="P134" s="20" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="Q134" s="20"/>
       <c r="R134" s="20"/>
@@ -5992,13 +5990,13 @@
     </row>
     <row r="135" spans="1:19" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="13" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C135" s="13" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D135" s="13" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E135" s="13" t="s">
         <v>90</v>
@@ -6013,13 +6011,13 @@
     <row r="136" spans="1:19" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="11"/>
       <c r="B136" s="11" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E136" s="11" t="s">
         <v>151</v>
@@ -6046,13 +6044,13 @@
     <row r="137" spans="1:19" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="11"/>
       <c r="B137" s="11" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E137" s="11" t="s">
         <v>151</v>
@@ -6079,10 +6077,10 @@
     <row r="138" spans="1:19" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="11"/>
       <c r="B138" s="11" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D138" s="11" t="s">
         <v>315</v>
@@ -6115,10 +6113,10 @@
         <v>314</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E139" s="11" t="s">
         <v>58</v>
@@ -6148,7 +6146,7 @@
         <v>315</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D140" s="11" t="s">
         <v>58</v>
@@ -6578,7 +6576,7 @@
     </row>
     <row r="156" spans="1:19" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B156" s="13" t="s">
         <v>164</v>
@@ -6611,7 +6609,7 @@
         <v>334</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="D157" s="11"/>
       <c r="E157" s="11"/>
@@ -6665,7 +6663,7 @@
         <v>889</v>
       </c>
       <c r="C159" s="11" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D159" s="11" t="s">
         <v>78</v>
@@ -6678,7 +6676,7 @@
       </c>
       <c r="G159" s="11"/>
       <c r="H159" s="11" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I159" s="11"/>
       <c r="J159" s="11"/>
@@ -7368,16 +7366,16 @@
     </row>
     <row r="185" spans="1:19" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="20" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B185" s="20" t="s">
+        <v>929</v>
+      </c>
+      <c r="C185" s="20" t="s">
+        <v>928</v>
+      </c>
+      <c r="D185" s="20" t="s">
         <v>931</v>
-      </c>
-      <c r="C185" s="20" t="s">
-        <v>930</v>
-      </c>
-      <c r="D185" s="20" t="s">
-        <v>933</v>
       </c>
       <c r="E185" s="20" t="s">
         <v>78</v>
@@ -7397,7 +7395,7 @@
       <c r="N185" s="20"/>
       <c r="O185" s="20"/>
       <c r="P185" s="20" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="Q185" s="20"/>
       <c r="R185" s="20"/>
@@ -8966,10 +8964,10 @@
     </row>
     <row r="267" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="20" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B267" s="20" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C267" s="22"/>
       <c r="D267" s="22"/>
@@ -8987,7 +8985,7 @@
       <c r="N267" s="22"/>
       <c r="O267" s="22"/>
       <c r="P267" s="22" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="Q267" s="20"/>
       <c r="R267" s="20"/>
@@ -9884,7 +9882,7 @@
         <v>60</v>
       </c>
       <c r="D336" s="12" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="E336" s="12" t="s">
         <v>61</v>
@@ -10220,7 +10218,7 @@
         <v>100</v>
       </c>
       <c r="D362" s="21" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="E362" s="21" t="s">
         <v>78</v>
@@ -11257,16 +11255,16 @@
     </row>
     <row r="447" spans="1:19" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A447" s="22" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B447" s="20" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C447" s="24" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D447" s="20" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E447" s="20" t="s">
         <v>78</v>
@@ -11284,7 +11282,7 @@
       <c r="N447" s="20"/>
       <c r="O447" s="20"/>
       <c r="P447" s="20" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="Q447" s="22"/>
       <c r="R447" s="23"/>
@@ -11725,7 +11723,7 @@
         <v>690</v>
       </c>
       <c r="C481" s="11" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F481" s="11" t="s">
         <v>3</v>
@@ -12097,7 +12095,7 @@
         <v>728</v>
       </c>
       <c r="C509" s="11" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="D509" s="11" t="s">
         <v>152</v>
@@ -12109,10 +12107,10 @@
         <v>3</v>
       </c>
       <c r="G509" s="19" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H509" s="11" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="P509" s="11" t="s">
         <v>150</v>
@@ -12388,7 +12386,7 @@
         <v>749</v>
       </c>
       <c r="C531" s="11" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="F531" s="11" t="s">
         <v>3</v>
@@ -13661,7 +13659,7 @@
         <v>860</v>
       </c>
       <c r="C637" s="11" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="D637" s="11" t="s">
         <v>597</v>
@@ -13881,10 +13879,10 @@
     <row r="655" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A655" s="13"/>
       <c r="B655" s="11" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C655" s="11" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D655" s="11" t="s">
         <v>302</v>
@@ -14157,7 +14155,7 @@
         <v>117</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -14179,7 +14177,7 @@
         <v>121</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>119</v>
@@ -14229,7 +14227,7 @@
         <v>129</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -14328,7 +14326,7 @@
         <v>886</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -14344,13 +14342,13 @@
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>